<commit_message>
fix: 1.5 decimal in perpherial blood
</commit_message>
<xml_diff>
--- a/dictionaries/methyl/1_5/1_5_peripheral-blood.xlsx
+++ b/dictionaries/methyl/1_5/1_5_peripheral-blood.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/Source/Visual/ds-dictionaries/dictionaries/methyl/1_4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/Source/Visual/ds-dictionaries/dictionaries/methyl/1_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7911CE33-675C-E445-B6D1-2FB463AD3361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E5C985-AF38-EC4E-8DB3-2FD84521E6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35500" yWindow="-6340" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>ageAcc3.Lee.refRPC</t>
-  </si>
-  <si>
-    <t>deceimal</t>
   </si>
   <si>
     <t>Age 1 - Lee refined RPC clock from methylclock: Useful for uncomplicated term pregnancies (e.g. gestational age &gt;36 weeks)</t>
@@ -1504,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IP44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1781,7 +1778,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1795,7 +1792,7 @@
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1809,7 +1806,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +1834,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1851,7 +1848,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1865,7 +1862,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1893,7 +1890,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1907,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1921,7 +1918,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1971,7 +1968,7 @@
         <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>4</v>

</xml_diff>